<commit_message>
Adicionados outros dados de tensão e deformação. Adicionado o angulo e o modulo de elasticidade no grafico e refatorei o código
</commit_message>
<xml_diff>
--- a/dadosEnsaioTracao.xlsx
+++ b/dadosEnsaioTracao.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Força</t>
+    <t xml:space="preserve">Força (N)</t>
   </si>
   <si>
-    <t xml:space="preserve">Derfomação</t>
+    <t xml:space="preserve">Comprimento(mm)</t>
   </si>
 </sst>
 </file>
@@ -34,7 +34,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -102,16 +102,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,128 +312,152 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>0</v>
+      <c r="B2" s="3" t="n">
+        <v>50.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>6.777</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0.0127</v>
+      <c r="A3" s="3" t="n">
+        <v>7.33</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>50.851</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>20.332</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.0381</v>
+      <c r="A4" s="4" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>50.902</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>33.886</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>0.0635</v>
+      <c r="A5" s="3" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>50.952</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>47.44</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.0889</v>
+      <c r="A6" s="3" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>51.003</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>52.489</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>0.127</v>
+      <c r="A7" s="3" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>51.054</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>52.489</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>0.2032</v>
+      <c r="A8" s="3" t="n">
+        <v>38.4</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>51.308</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>53.379</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>0.508</v>
+      <c r="A9" s="3" t="n">
+        <v>41.3</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>51.816</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>73.84</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>1.016</v>
+      <c r="A10" s="3" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>52.832</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>88.964</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>2.54</v>
+      <c r="A11" s="3" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>53.848</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>95.637</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>7.112</v>
+      <c r="A12" s="3" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>54.864</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>86.74</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>10.16</v>
+      <c r="A13" s="3" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>55.88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>82.292</v>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>11.684</v>
+      <c r="A14" s="3" t="n">
+        <v>46.1</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>56.896</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>57.658</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>58.42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>36.4</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>59.182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Acrecentado funções para plotagem de novos dados
</commit_message>
<xml_diff>
--- a/dadosEnsaioTracao.xlsx
+++ b/dadosEnsaioTracao.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Força (N)</t>
+    <t xml:space="preserve">kN</t>
   </si>
   <si>
-    <t xml:space="preserve">Comprimento(mm)</t>
+    <t xml:space="preserve">mm</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>